<commit_message>
Addition of PWM Blend
</commit_message>
<xml_diff>
--- a/CustomHomeRJ45GPIOConfigurations.xlsx
+++ b/CustomHomeRJ45GPIOConfigurations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Hobbies\GitHub\HomeAutomationControlSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32676A9-B949-454D-976D-090C5F2147C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA68D7D-27D1-4F94-83C8-B3AA2CFD8A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="315" windowWidth="38670" windowHeight="21420" xr2:uid="{16AC328A-FD66-42D0-B89E-63D872D627A6}"/>
+    <workbookView xWindow="-63468" yWindow="-1884" windowWidth="17496" windowHeight="30480" xr2:uid="{16AC328A-FD66-42D0-B89E-63D872D627A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>RJ45 as TypeB</t>
   </si>
@@ -191,6 +191,21 @@
   </si>
   <si>
     <t>SR04_RX</t>
+  </si>
+  <si>
+    <t>ESP32 Type A</t>
+  </si>
+  <si>
+    <t>6P</t>
+  </si>
+  <si>
+    <t>I2D</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>UART_TX will be dominant colour, as its important to identify output from esp pin (note this is transmit out of esp, thus RX from peripherials connect to this)</t>
   </si>
 </sst>
 </file>
@@ -649,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699E15B7-7E82-4833-846A-CE360D2701DA}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,10 +767,13 @@
         <v>13</v>
       </c>
       <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" t="s">
-        <v>15</v>
+      <c r="K3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -945,6 +963,72 @@
         <v>51</v>
       </c>
     </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B17:J17"/>

</xml_diff>